<commit_message>
Small edits to large communities experiment
</commit_message>
<xml_diff>
--- a/experiments/largest-communities/processed.xlsx
+++ b/experiments/largest-communities/processed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Self\Repositories\wikipedia-separation\experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Self\Repositories\wikipedia-separation\experiments\largest-communities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E3C0E51-0FD8-4753-864E-ED61B925FDA5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CAB8CC-F03F-4189-8CBE-8C26DE02DDE5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23865" windowHeight="7980" activeTab="7" xr2:uid="{B5426E11-8EF5-4392-BC0D-BCC1B56745FB}"/>
   </bookViews>
@@ -154,6 +154,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Path length for 100 shortest paths between random nodes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -326,6 +351,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Amount of large communities blocked</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -388,6 +468,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> # nodes on path </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9519,7 +9659,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>